<commit_message>
Update carbon budget scenarios and run definitions
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget-CAP24_250MT-new.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget-CAP24_250MT-new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\times-ireland-model-2019-2023calib\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\times-ireland-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C28F0B-9A1F-45D0-9FB2-401DB8666936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6449E3-E6EB-4CED-AE08-9BA88B7F70C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="124">
   <si>
     <t>LimType</t>
   </si>
@@ -529,6 +529,9 @@
   </si>
   <si>
     <t>2021-2050</t>
+  </si>
+  <si>
+    <t>Suleimenov Bakytzhan (UCC, bsuleimenov@ucc.ie)</t>
   </si>
 </sst>
 </file>
@@ -5120,7 +5123,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="39" fmlaLink="$A$4" fmlaRange="$A$5:$A$7" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="39" fmlaLink="$A$4" fmlaRange="$A$5:$A$7" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5396,7 +5399,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>21771</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -5786,20 +5789,20 @@
   <dimension ref="A1:Z99"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B26" sqref="B26:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="4" width="21.69140625" customWidth="1"/>
-    <col min="5" max="6" width="14.07421875" customWidth="1"/>
-    <col min="7" max="7" width="12.07421875" customWidth="1"/>
-    <col min="8" max="10" width="8.07421875" customWidth="1"/>
-    <col min="11" max="11" width="9.69140625" customWidth="1"/>
-    <col min="12" max="12" width="8.07421875" customWidth="1"/>
+    <col min="1" max="4" width="21.7265625" customWidth="1"/>
+    <col min="5" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="8" max="10" width="8.08984375" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" customWidth="1"/>
+    <col min="12" max="12" width="8.08984375" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.3046875" customWidth="1"/>
-    <col min="15" max="15" width="13.3046875" customWidth="1"/>
+    <col min="14" max="14" width="11.26953125" customWidth="1"/>
+    <col min="15" max="15" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -6525,7 +6528,7 @@
         <v>95</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
@@ -8637,36 +8640,36 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.07421875" customWidth="1"/>
-    <col min="2" max="2" width="11.69140625" customWidth="1"/>
-    <col min="3" max="3" width="3.07421875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.53515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.84375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.84375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.3046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.69140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.53515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.07421875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.69140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.53515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.3046875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.69140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.07421875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.69140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.53515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.84375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.69140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.84375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.53515625" customWidth="1"/>
-    <col min="25" max="25" width="6.69140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.07421875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="3" max="3" width="3.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.54296875" customWidth="1"/>
+    <col min="25" max="25" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.08984375" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.69140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.69140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:30">
@@ -8676,116 +8679,116 @@
       </c>
       <c r="D3" s="1" t="str" cm="1">
         <f t="array" ref="D3">IF(LEFT(INDEX(D5:D7,$A$4),1)&lt;&gt;"*",INDEX(D5:D7,$A$4),"")</f>
-        <v>National</v>
+        <v/>
       </c>
       <c r="E3" s="1" t="str" cm="1">
         <f t="array" ref="E3">IF(LEFT(INDEX(E5:E7,$A$4),1)&lt;&gt;"*",INDEX(E5:E7,$A$4),"")</f>
-        <v>IE-CW</v>
+        <v/>
       </c>
       <c r="F3" s="1" t="str" cm="1">
         <f t="array" ref="F3">IF(LEFT(INDEX(F5:F7,$A$4),1)&lt;&gt;"*",INDEX(F5:F7,$A$4),"")</f>
-        <v>IE-D</v>
+        <v/>
       </c>
       <c r="G3" s="1" t="str" cm="1">
         <f t="array" ref="G3">IF(LEFT(INDEX(G5:G7,$A$4),1)&lt;&gt;"*",INDEX(G5:G7,$A$4),"")</f>
-        <v>IE-KE</v>
+        <v/>
       </c>
       <c r="H3" s="1" t="str" cm="1">
         <f t="array" ref="H3">IF(LEFT(INDEX(H5:H7,$A$4),1)&lt;&gt;"*",INDEX(H5:H7,$A$4),"")</f>
-        <v>IE-KK</v>
+        <v/>
       </c>
       <c r="I3" s="1" t="str" cm="1">
         <f t="array" ref="I3">IF(LEFT(INDEX(I5:I7,$A$4),1)&lt;&gt;"*",INDEX(I5:I7,$A$4),"")</f>
-        <v>IE-LS</v>
+        <v/>
       </c>
       <c r="J3" s="1" t="str" cm="1">
         <f t="array" ref="J3">IF(LEFT(INDEX(J5:J7,$A$4),1)&lt;&gt;"*",INDEX(J5:J7,$A$4),"")</f>
-        <v>IE-LD</v>
+        <v/>
       </c>
       <c r="K3" s="1" t="str" cm="1">
         <f t="array" ref="K3">IF(LEFT(INDEX(K5:K7,$A$4),1)&lt;&gt;"*",INDEX(K5:K7,$A$4),"")</f>
-        <v>IE-LH</v>
+        <v/>
       </c>
       <c r="L3" s="1" t="str" cm="1">
         <f t="array" ref="L3">IF(LEFT(INDEX(L5:L7,$A$4),1)&lt;&gt;"*",INDEX(L5:L7,$A$4),"")</f>
-        <v>IE-MH</v>
+        <v/>
       </c>
       <c r="M3" s="1" t="str" cm="1">
         <f t="array" ref="M3">IF(LEFT(INDEX(M5:M7,$A$4),1)&lt;&gt;"*",INDEX(M5:M7,$A$4),"")</f>
-        <v>IE-OY</v>
+        <v/>
       </c>
       <c r="N3" s="1" t="str" cm="1">
         <f t="array" ref="N3">IF(LEFT(INDEX(N5:N7,$A$4),1)&lt;&gt;"*",INDEX(N5:N7,$A$4),"")</f>
-        <v>IE-WH</v>
+        <v/>
       </c>
       <c r="O3" s="1" t="str" cm="1">
         <f t="array" ref="O3">IF(LEFT(INDEX(O5:O7,$A$4),1)&lt;&gt;"*",INDEX(O5:O7,$A$4),"")</f>
-        <v>IE-WX</v>
+        <v/>
       </c>
       <c r="P3" s="1" t="str" cm="1">
         <f t="array" ref="P3">IF(LEFT(INDEX(P5:P7,$A$4),1)&lt;&gt;"*",INDEX(P5:P7,$A$4),"")</f>
-        <v>IE-WW</v>
+        <v/>
       </c>
       <c r="Q3" s="1" t="str" cm="1">
         <f t="array" ref="Q3">IF(LEFT(INDEX(Q5:Q7,$A$4),1)&lt;&gt;"*",INDEX(Q5:Q7,$A$4),"")</f>
-        <v>IE-CE</v>
+        <v/>
       </c>
       <c r="R3" s="1" t="str" cm="1">
         <f t="array" ref="R3">IF(LEFT(INDEX(R5:R7,$A$4),1)&lt;&gt;"*",INDEX(R5:R7,$A$4),"")</f>
-        <v>IE-CO</v>
+        <v/>
       </c>
       <c r="S3" s="1" t="str" cm="1">
         <f t="array" ref="S3">IF(LEFT(INDEX(S5:S7,$A$4),1)&lt;&gt;"*",INDEX(S5:S7,$A$4),"")</f>
-        <v>IE-KY</v>
+        <v/>
       </c>
       <c r="T3" s="1" t="str" cm="1">
         <f t="array" ref="T3">IF(LEFT(INDEX(T5:T7,$A$4),1)&lt;&gt;"*",INDEX(T5:T7,$A$4),"")</f>
-        <v>IE-LK</v>
+        <v/>
       </c>
       <c r="U3" s="1" t="str" cm="1">
         <f t="array" ref="U3">IF(LEFT(INDEX(U5:U7,$A$4),1)&lt;&gt;"*",INDEX(U5:U7,$A$4),"")</f>
-        <v>IE-TA</v>
+        <v/>
       </c>
       <c r="V3" s="1" t="str" cm="1">
         <f t="array" ref="V3">IF(LEFT(INDEX(V5:V7,$A$4),1)&lt;&gt;"*",INDEX(V5:V7,$A$4),"")</f>
-        <v>IE-WD</v>
+        <v/>
       </c>
       <c r="W3" s="1" t="str" cm="1">
         <f t="array" ref="W3">IF(LEFT(INDEX(W5:W7,$A$4),1)&lt;&gt;"*",INDEX(W5:W7,$A$4),"")</f>
-        <v>IE-G</v>
+        <v/>
       </c>
       <c r="X3" s="1" t="str" cm="1">
         <f t="array" ref="X3">IF(LEFT(INDEX(X5:X7,$A$4),1)&lt;&gt;"*",INDEX(X5:X7,$A$4),"")</f>
-        <v>IE-LM</v>
+        <v/>
       </c>
       <c r="Y3" s="1" t="str" cm="1">
         <f t="array" ref="Y3">IF(LEFT(INDEX(Y5:Y7,$A$4),1)&lt;&gt;"*",INDEX(Y5:Y7,$A$4),"")</f>
-        <v>IE-MO</v>
+        <v/>
       </c>
       <c r="Z3" s="1" t="str" cm="1">
         <f t="array" ref="Z3">IF(LEFT(INDEX(Z5:Z7,$A$4),1)&lt;&gt;"*",INDEX(Z5:Z7,$A$4),"")</f>
-        <v>IE-RN</v>
+        <v/>
       </c>
       <c r="AA3" s="1" t="str" cm="1">
         <f t="array" ref="AA3">IF(LEFT(INDEX(AA5:AA7,$A$4),1)&lt;&gt;"*",INDEX(AA5:AA7,$A$4),"")</f>
-        <v>IE-SO</v>
+        <v/>
       </c>
       <c r="AB3" s="1" t="str" cm="1">
         <f t="array" ref="AB3">IF(LEFT(INDEX(AB5:AB7,$A$4),1)&lt;&gt;"*",INDEX(AB5:AB7,$A$4),"")</f>
-        <v>IE-CN</v>
+        <v/>
       </c>
       <c r="AC3" s="1" t="str" cm="1">
         <f t="array" ref="AC3">IF(LEFT(INDEX(AC5:AC7,$A$4),1)&lt;&gt;"*",INDEX(AC5:AC7,$A$4),"")</f>
-        <v>IE-DL</v>
+        <v/>
       </c>
       <c r="AD3" s="1" t="str" cm="1">
         <f t="array" ref="AD3">IF(LEFT(INDEX(AD5:AD7,$A$4),1)&lt;&gt;"*",INDEX(AD5:AD7,$A$4),"")</f>
-        <v>IE-MN</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -9379,7 +9382,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>21771</xdr:colOff>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -9399,18 +9402,18 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B4:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.07421875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9682,23 +9685,23 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="28.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.69140625" customWidth="1"/>
-    <col min="7" max="7" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.53515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.07421875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -9841,8 +9844,8 @@
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="str">
-        <f>VLOOKUP($B$5, config!$B$4:$F$14,3,FALSE) &amp; "_Single"</f>
-        <v>UC_CB_250_Mt_2021-2030_Single</v>
+        <f>"\I:"&amp;VLOOKUP($B$5, config!$B$4:$F$14,3,FALSE) &amp; "_Single"</f>
+        <v>\I:UC_CB_250_Mt_2021-2030_Single</v>
       </c>
       <c r="C9" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
@@ -10044,19 +10047,19 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="33.07421875" customWidth="1"/>
+    <col min="2" max="2" width="33.08984375" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.53515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.07421875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.3046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -10067,7 +10070,7 @@
     <row r="2" spans="1:12">
       <c r="B2" s="9" t="str">
         <f>"UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
-        <v>UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+        <v xml:space="preserve">UC_Sets: R_S: </v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -10078,7 +10081,7 @@
     <row r="4" spans="1:12">
       <c r="H4" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","UC_T","")</f>
-        <v>UC_T</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -10403,12 +10406,12 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.07421875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.07421875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
@@ -10438,7 +10441,7 @@
       </c>
       <c r="H3" s="16" t="str">
         <f>Regions!D3</f>
-        <v>National</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="2:9">

</xml_diff>